<commit_message>
curves : st.errors added (scripts)
</commit_message>
<xml_diff>
--- a/output/curves/dsc.1.uvvis/semicolon/output.xlsx
+++ b/output/curves/dsc.1.uvvis/semicolon/output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">label</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">st.error</t>
   </si>
   <si>
     <t xml:space="preserve">215</t>
@@ -4680,204 +4683,246 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0537283449373566</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.275127271354307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.290046976197438</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.27042286264458</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0767744540860477</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.370531469823652</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.352491419732517</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5.56389026214797</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0167820231539354</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0124547632532439</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0111468039273016</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0072026173799019</v>
       </c>
     </row>
     <row r="14">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E14"/>
     </row>
     <row r="15">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E15"/>
     </row>
     <row r="16">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4898,12 +4943,12 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
         <v>59.6388602726335</v>
@@ -4911,7 +4956,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
         <v>18.117480405815</v>
@@ -4919,7 +4964,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="n">
         <v>17.991544420833</v>
@@ -4927,7 +4972,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="n">
         <v>4.92638597306541</v>
@@ -4952,22 +4997,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -16972,10 +17017,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
@@ -22285,13 +22330,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">

</xml_diff>